<commit_message>
added Word and Excel
</commit_message>
<xml_diff>
--- a/Daily Project Journal.xlsx
+++ b/Daily Project Journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\PythonAI\LearnH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46444F44-87A7-459C-8A85-497867FB08BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8EFC77-19AD-4B02-8338-372579A3498E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3160" windowWidth="19200" windowHeight="8120" tabRatio="877" activeTab="1" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="877" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
   </bookViews>
   <sheets>
     <sheet name="DailyNotes" sheetId="6" r:id="rId1"/>
@@ -44,35 +44,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="98">
   <si>
     <t>List of capabilities</t>
   </si>
   <si>
-    <t>- Read/input text from any PDF</t>
-  </si>
-  <si>
-    <t>- Build knowledge from each PDF. Retain that state.</t>
-  </si>
-  <si>
-    <t>- Verify with user whether output is accurate.</t>
-  </si>
-  <si>
-    <t>- Refine knowledge through user-input.</t>
-  </si>
-  <si>
-    <t>- Verify/vet/re-learn from user-input.</t>
-  </si>
-  <si>
     <t>-- This must be able to cross-reference at least three other sources that come to similar conclusions</t>
   </si>
   <si>
     <t>- Think like succesful energy investors</t>
   </si>
   <si>
-    <t>- Award tokens for flagging errors and suggesting new, community-accepted answers.</t>
-  </si>
-  <si>
     <t>- Set base knowledge of Hydrogen</t>
   </si>
   <si>
@@ -211,9 +193,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>- Given string of questions, recommend further research, calculations, analysis.</t>
-  </si>
-  <si>
     <t>- Refine contractor's SOW after spend a few days working on algo myself.</t>
   </si>
   <si>
@@ -268,9 +247,6 @@
     <t>How to change the sources the LLM uses?</t>
   </si>
   <si>
-    <t>- Add other documents that complement H2 TEA - (solar, wind, CCUS, biofuels, geothermal, nuclear, PPAs, incentives, legal, transportation, storage, ...)</t>
-  </si>
-  <si>
     <t>- Get Pinecone and Estuary setup for vectorstor DB and read two articles on Chrome. Research more into vectorstores</t>
   </si>
   <si>
@@ -302,6 +278,66 @@
   </si>
   <si>
     <t>3) Build Web app interface</t>
+  </si>
+  <si>
+    <t>Continued working on  input file for Estuary. Created a JSON and got feedback from Jenny on what to do next</t>
+  </si>
+  <si>
+    <t>rest the mind</t>
+  </si>
+  <si>
+    <t>Finish connection to estuary and contractor document</t>
+  </si>
+  <si>
+    <t>- Read/input text from any PDF, Excel/CSV, URL</t>
+  </si>
+  <si>
+    <t>- Add other documents that complement H2 TEA - (oil &amp; gas focused first:  CCUS, biofuels, RECs/PPAs, incentives, legal, transportation, storage, solar, wind, geothermal, nuclear...)</t>
+  </si>
+  <si>
+    <t>Briefly reserached developerts -&gt; Need to identify at least 5.</t>
+  </si>
+  <si>
+    <t>-- Li-ion batteries</t>
+  </si>
+  <si>
+    <t>-- Carbon capture, utilization, and sequestration</t>
+  </si>
+  <si>
+    <t>-- Refine knowledge through user feedback which is in the form of them providing PDFs or URLs</t>
+  </si>
+  <si>
+    <t>-- Verify/vet/re-learn from user-input.</t>
+  </si>
+  <si>
+    <t>- Build knowledge from all inputs and retain that state through entire interaction with user.</t>
+  </si>
+  <si>
+    <t>- Given string of questions, recommend other relevant prompts.</t>
+  </si>
+  <si>
+    <t>-- Better material on policy and credits (45V and 45Q)</t>
+  </si>
+  <si>
+    <t>- Consider other topics. Should somehow be very relevant to hydrogen such as competiting technologies.</t>
+  </si>
+  <si>
+    <t>- Verify with user whether output is accurate and update future answers.</t>
+  </si>
+  <si>
+    <t>Bold: Key activity map activities</t>
+  </si>
+  <si>
+    <t>-- After each prompt, provide a list of three relevant prompts</t>
+  </si>
+  <si>
+    <t>-- Award tokens for flagging errors and suggesting new, community-accepted answers.</t>
+  </si>
+  <si>
+    <t>- Other possible activities in MVP:</t>
+  </si>
+  <si>
+    <t>Worked on estuary connection, still no luck. Added to activity map.</t>
   </si>
 </sst>
 </file>
@@ -354,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -380,6 +416,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,13 +808,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C65F3B7-4679-46BB-9C6C-4439D434827C}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -786,230 +829,288 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
-        <v>45105</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="4">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="13">
+        <v>45110</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="13">
+        <v>45109</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="13">
+        <v>45108</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="13">
+        <v>45107</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="13">
         <v>45106</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <v>45104</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
-        <v>45103</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>45102</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="4">
-        <v>45110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
-        <v>45102</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>57</v>
+      <c r="B6" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="4">
-        <v>45117</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>45101</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>50</v>
+        <v>45105</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="D7" s="4">
+        <v>45106</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
+        <v>45104</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>45103</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>45102</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="4">
+        <v>45110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>45102</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="4">
+        <v>45117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
         <v>45101</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="B12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>45101</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="10">
+        <v>45101</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="10">
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="10">
         <v>45101</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="10">
-        <v>45101</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>45100</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>47</v>
+      <c r="B16" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>45099</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>37</v>
+        <v>45100</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
         <v>45099</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
+      <c r="B22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>45099</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G7:G10 C1:D1048576">
+  <conditionalFormatting sqref="G12:G15 C1:D1048576">
     <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
@@ -1031,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06015F9D-4AF7-453E-80C4-3DF1FC0EE8F4}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1043,92 +1144,92 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B1" s="12"/>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B5" s="12"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1154,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47DD1B2-F515-4063-A283-1EBFB574D93C}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="B1:C1"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1169,110 +1270,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>45122</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
+      <c r="A5" s="16" t="s">
+        <v>88</v>
+      </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
+      <c r="A6" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1"/>
+    <row r="11" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="16"/>
+    </row>
+    <row r="12" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="16"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>8</v>
+      <c r="A13" s="16" t="s">
+        <v>96</v>
       </c>
       <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>5</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1295,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1303,7 +1434,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1323,22 +1454,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1359,12 +1490,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1384,47 +1515,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1447,37 +1578,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates. New Python script to test Materialization
</commit_message>
<xml_diff>
--- a/Daily Project Journal.xlsx
+++ b/Daily Project Journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\PythonAI\LearnH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA45F66B-C7F7-4113-B756-6ED0DB15189C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2242FE45-9A17-4090-A1FF-A6859B4C910A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="877" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
+    <workbookView xWindow="0" yWindow="4600" windowWidth="19130" windowHeight="6740" tabRatio="877" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
   </bookViews>
   <sheets>
     <sheet name="DailyNotes" sheetId="6" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
   <si>
     <t>List of capabilities</t>
   </si>
@@ -348,6 +348,15 @@
   </si>
   <si>
     <t>Tried Jenny's suggestions. Responded with email with my error messages and asked her to setup for me. Worked more on contractor's SOW. Think it is now near final. Need to focus shift to the AI model now to make sure it offers more value than ChatGPT.</t>
+  </si>
+  <si>
+    <t>- Current Knowledge of (Policies, funding announcements, projects, …)</t>
+  </si>
+  <si>
+    <t>-- Data sources: DOE RSS feeds, FOAs, useful public dataset</t>
+  </si>
+  <si>
+    <t>Jenny fixed my Estuary schema. Materialization worked and published! However, first query gave back strange answer</t>
   </si>
 </sst>
 </file>
@@ -2479,13 +2488,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C65F3B7-4679-46BB-9C6C-4439D434827C}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2521,24 +2530,24 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>45112</v>
+        <v>45113</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>45111</v>
+        <v>45112</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>39</v>
@@ -2547,161 +2556,161 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>45110</v>
+        <v>45111</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>45109</v>
+        <v>45110</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>45108</v>
+        <v>45109</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
+        <v>45108</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>45107</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B8" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
-        <v>45106</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
+        <v>45106</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
         <v>45105</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="4">
-        <v>45106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
-        <v>45104</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="4">
+        <v>45106</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>45103</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>71</v>
+        <v>45104</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>45102</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>45103</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="C12" t="s">
         <v>42</v>
-      </c>
-      <c r="D12" s="4">
-        <v>45110</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>45102</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>50</v>
+      <c r="B13" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="C13" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="4">
-        <v>45117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>45110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>45101</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>44</v>
+        <v>45102</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="C14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D14" s="4">
+        <v>45117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>45101</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>45101</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="10">
-        <v>45101</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>48</v>
-      </c>
+      <c r="D16" s="9"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -2709,30 +2718,31 @@
         <v>45101</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>48</v>
       </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
+    <row r="18" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="10">
+        <v>45101</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>45100</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>34</v>
+      <c r="B19" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -2743,7 +2753,7 @@
         <v>45100</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>39</v>
@@ -2754,10 +2764,10 @@
         <v>45100</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -2765,10 +2775,10 @@
         <v>45100</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -2776,21 +2786,21 @@
         <v>45100</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <v>45099</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>31</v>
+        <v>45100</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -2798,14 +2808,25 @@
         <v>45099</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="26" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4">
+        <v>45099</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G14:G17 C1:D1048576">
+  <conditionalFormatting sqref="G15:G18 C1:D1048576">
     <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
@@ -3004,10 +3025,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47DD1B2-F515-4063-A283-1EBFB574D93C}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3050,120 +3071,148 @@
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="1"/>
+        <v>101</v>
+      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" s="12"/>
-    </row>
-    <row r="13" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="12"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
-        <v>96</v>
       </c>
       <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>95</v>
       </c>
       <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>91</v>
-      </c>
+    <row r="17" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="12"/>
+    </row>
+    <row r="19" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="12"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="A20" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>85</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B21" s="1"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated BP and PD
</commit_message>
<xml_diff>
--- a/Daily Project Journal.xlsx
+++ b/Daily Project Journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\PythonAI\LearnH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17F965F-C38C-4A17-8630-8C60D7DC32FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45114052-97D3-4AFB-B5EF-664AC1A30D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="877" activeTab="4" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="11260" tabRatio="877" activeTab="4" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
   </bookViews>
   <sheets>
     <sheet name="MVPFeatures" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="121">
   <si>
     <t>List of capabilities</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>Remade connection to Pinecone in the script. Not sure GPT is giving back proper results so trying to make sure the LLM is in fact pulling from the knowledge base in Pinecone's vectorDB. Next step is to verify this and then start to break down accuracy of questions</t>
+  </si>
+  <si>
+    <t>Created pitch deck, updated business plan, thought more about Year 2.</t>
   </si>
 </sst>
 </file>
@@ -655,6 +658,71 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>246529</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>37353</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="110" name="Rectangle 109">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4D3331A-C120-AC26-AE80-2335F9A887C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9435353" y="2958353"/>
+          <a:ext cx="2241176" cy="3690471"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:alpha val="20000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>216648</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -1489,14 +1557,14 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>512483</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>183776</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1507</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>491192</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>143809</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76436</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1511,8 +1579,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9701307" y="3172011"/>
-          <a:ext cx="1816473" cy="1267386"/>
+          <a:off x="9684705" y="3100072"/>
+          <a:ext cx="1813154" cy="1350808"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1556,7 +1624,7 @@
                 <a:schemeClr val="tx2"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Users awarded larger amount of tokens once three</a:t>
+            <a:t>Users awarded larger amount of tokens (or karma) once three</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -1748,15 +1816,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>190312</xdr:colOff>
+      <xdr:colOff>190865</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>149039</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>195544</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>183776</xdr:rowOff>
+      <xdr:colOff>196097</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1507</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1774,8 +1842,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="10604312" y="2203451"/>
-          <a:ext cx="5232" cy="968560"/>
+          <a:off x="10586050" y="2153993"/>
+          <a:ext cx="5232" cy="946079"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1804,13 +1872,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>195544</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>143809</xdr:rowOff>
+      <xdr:colOff>196097</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>201334</xdr:colOff>
+      <xdr:colOff>201888</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>104216</xdr:rowOff>
     </xdr:to>
@@ -1830,8 +1898,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="10609544" y="4439397"/>
-          <a:ext cx="5790" cy="894231"/>
+          <a:off x="10591282" y="4450880"/>
+          <a:ext cx="5791" cy="756855"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1974,13 +2042,13 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>138578</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>70410</xdr:rowOff>
+      <xdr:rowOff>93757</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>512483</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>93756</xdr:rowOff>
+      <xdr:rowOff>130106</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1997,9 +2065,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="9327402" y="3805704"/>
-          <a:ext cx="373905" cy="23346"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9310800" y="3739127"/>
+          <a:ext cx="373905" cy="36349"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2415,71 +2483,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>246529</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>156882</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>37353</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="110" name="Rectangle 109">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4D3331A-C120-AC26-AE80-2335F9A887C2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9435353" y="2958353"/>
-          <a:ext cx="2241176" cy="3690471"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:alpha val="20000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -2965,13 +2968,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>109819</xdr:colOff>
+      <xdr:colOff>86300</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>88901</xdr:rowOff>
+      <xdr:rowOff>170510</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>529666</xdr:colOff>
+      <xdr:colOff>506147</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>177675</xdr:rowOff>
     </xdr:to>
@@ -2988,8 +2991,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6248152" y="8185151"/>
-          <a:ext cx="1033681" cy="268691"/>
+          <a:off x="6201115" y="8372593"/>
+          <a:ext cx="1031328" cy="189434"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3028,13 +3031,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>72340</xdr:colOff>
+      <xdr:colOff>142896</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>95003</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>493433</xdr:colOff>
+      <xdr:colOff>563989</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>3861</xdr:rowOff>
     </xdr:to>
@@ -3051,8 +3054,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4983007" y="7831420"/>
-          <a:ext cx="1034926" cy="268691"/>
+          <a:off x="5034748" y="7932549"/>
+          <a:ext cx="1032574" cy="273395"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3217,15 +3220,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>125381</xdr:colOff>
+      <xdr:colOff>61881</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>99358</xdr:rowOff>
+      <xdr:rowOff>64676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>407518</xdr:colOff>
+      <xdr:colOff>493889</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>20169</xdr:rowOff>
+      <xdr:rowOff>135232</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3240,8 +3243,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6263714" y="7835775"/>
-          <a:ext cx="895971" cy="280644"/>
+          <a:off x="6176696" y="7902222"/>
+          <a:ext cx="1043489" cy="435093"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3268,6 +3271,14 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>integrated</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> systems</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -3472,15 +3483,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>435533</xdr:colOff>
+      <xdr:colOff>417894</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>90641</xdr:rowOff>
+      <xdr:rowOff>131799</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>93132</xdr:colOff>
+      <xdr:colOff>75493</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>93131</xdr:rowOff>
+      <xdr:rowOff>134289</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3495,8 +3506,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="435533" y="8546724"/>
-          <a:ext cx="1499099" cy="362324"/>
+          <a:off x="417894" y="8698419"/>
+          <a:ext cx="1492043" cy="367027"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6814,8 +6825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC1441B-92AB-4D26-A8D1-26583D2CCC09}">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8067,13 +8078,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C65F3B7-4679-46BB-9C6C-4439D434827C}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8109,60 +8120,60 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>45122</v>
+        <v>45123</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>45121</v>
+        <v>45122</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
+        <v>45121</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>45120</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B5" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>45119</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>45118</v>
+        <v>45119</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -8171,10 +8182,10 @@
     </row>
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>45117</v>
+        <v>45118</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
         <v>33</v>
@@ -8183,10 +8194,10 @@
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>45116</v>
+        <v>45117</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -8195,58 +8206,58 @@
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>45115</v>
+        <v>45116</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
+        <v>45115</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
         <v>45114</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B11" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
         <v>45113</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B12" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
-        <v>45112</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>45111</v>
+        <v>45112</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
@@ -8255,22 +8266,22 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>45110</v>
+        <v>45111</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <v>45109</v>
+        <v>45110</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>33</v>
@@ -8279,168 +8290,169 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>45108</v>
+        <v>45109</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" t="s">
-        <v>36</v>
+        <v>70</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
+        <v>45108</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
         <v>45107</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B18" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
         <v>45106</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B19" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
-        <v>45105</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="4">
-        <v>45106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>45104</v>
+        <v>45105</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="4">
+        <v>45106</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>45103</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>65</v>
+        <v>45104</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <v>45102</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>43</v>
+        <v>45103</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="C22" t="s">
         <v>36</v>
-      </c>
-      <c r="D22" s="4">
-        <v>45110</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>45102</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>44</v>
+      <c r="B23" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="C23" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="4">
-        <v>45117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>45110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <v>45101</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>38</v>
+        <v>45102</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="C24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D24" s="4">
+        <v>45117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>45101</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="4">
+        <v>45101</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="10">
+      <c r="D26" s="9"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="10">
         <v>45101</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B27" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="4">
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
         <v>45101</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>33</v>
-      </c>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>45100</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>28</v>
+      <c r="B29" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="C29" t="s">
         <v>33</v>
@@ -8451,7 +8463,7 @@
         <v>45100</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
         <v>33</v>
@@ -8462,10 +8474,10 @@
         <v>45100</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -8473,10 +8485,10 @@
         <v>45100</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -8484,21 +8496,21 @@
         <v>45100</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
-        <v>45099</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>25</v>
+        <v>45100</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -8506,14 +8518,25 @@
         <v>45099</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="36" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="4">
+        <v>45099</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G24:G27 C1:D1048576">
+  <conditionalFormatting sqref="G25:G28 C1:D1048576">
     <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>$G$1</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated deck, excel, code
</commit_message>
<xml_diff>
--- a/Daily Project Journal.xlsx
+++ b/Daily Project Journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\PythonAI\LearnH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7945C60-FE54-458D-AD23-D530FB3EB9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29847FD5-4732-40E7-A2C8-A6EBDA06513F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="877" activeTab="5" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="877" activeTab="1" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
   </bookViews>
   <sheets>
     <sheet name="MVPFeatures" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="129">
   <si>
     <t>List of capabilities</t>
   </si>
@@ -524,20 +524,20 @@
     <t>Worked on NDA. Started customer focus group on customer survey. Updated pitch deck. Thinking I should either focus on larger customer segment, or dive deeper into niche.</t>
   </si>
   <si>
-    <t>No 2</t>
-  </si>
-  <si>
-    <t>Wingman</t>
-  </si>
-  <si>
-    <t>wingbot</t>
+    <t>C.H.E.W.I.E.</t>
+  </si>
+  <si>
+    <t>Worked on Pitch Deck, use cases, researched pre-seed vs. seed funding. Hongtai mentioned interest in supporting. Has experience in product development and pipeline needed to support product.</t>
+  </si>
+  <si>
+    <t>Came up with CHEWIE. Filled in use cases.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,6 +586,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="30"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -619,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -662,6 +670,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4006,13 +4015,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4071,13 +4080,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4147,13 +4156,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>536015</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>282015</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4211,13 +4220,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4279,13 +4288,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>374650</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4347,13 +4356,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>219261</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>125133</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28761</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>144182</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4410,13 +4419,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>418353</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>102722</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>448234</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>149413</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4473,13 +4482,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9338</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4526,13 +4535,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>260724</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>116541</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>9339</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>116541</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4579,13 +4588,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>413124</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>72091</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>476624</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>18677</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4647,13 +4656,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>599141</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>20170</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>466912</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>102719</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4715,13 +4724,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>501650</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4768,13 +4777,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>491938</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>76946</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>569633</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>746</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4837,13 +4846,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>36233</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>375770</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>36793</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4893,13 +4902,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>168088</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>46692</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4946,13 +4955,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>584199</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>106456</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>100106</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5010,13 +5019,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5063,13 +5072,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5127,13 +5136,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>326839</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>46691</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>494926</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>46691</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5180,13 +5189,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>211045</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>93755</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>566645</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>87406</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5244,13 +5253,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>375024</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>141568</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>222623</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>43703</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5326,13 +5335,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>46318</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>178547</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>135218</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>29882</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5404,13 +5413,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5468,13 +5477,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>550956</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>54162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>150905</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>60512</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5536,13 +5545,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5600,13 +5609,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>103094</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>29509</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>58644</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>184524</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5668,13 +5677,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>223744</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>29509</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>583079</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>152774</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5732,13 +5741,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>185644</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>61259</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>602130</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>80309</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5795,13 +5804,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>341081</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>176241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>93431</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>105432</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5859,14 +5868,14 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>575968</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>99718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>269214</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>98252</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>98253</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5912,13 +5921,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>428725</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>158005</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>177340</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>151654</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5976,14 +5985,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>96127</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>73858</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>396358</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>72392</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>72393</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6029,13 +6038,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>14252</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>104130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>485590</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>149412</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6094,17 +6103,17 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>233185</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>186722</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>233545</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>317</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>318</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="21" name="Ink 20">
@@ -6123,7 +6132,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="21" name="Ink 20">
@@ -6159,13 +6168,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>37350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>196104</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>140071</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6227,13 +6236,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>329825</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>31002</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>208429</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>133722</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6290,13 +6299,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>560294</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>140071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>560295</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6345,13 +6354,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>560295</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>133722</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>572620</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>37350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6401,13 +6410,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>569634</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>70595</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>392207</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>140074</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6465,13 +6474,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>544607</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>157627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>367180</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>81426</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6529,13 +6538,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>566084</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>186764</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>572620</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>31002</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6585,13 +6594,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>43331</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>39218</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>472889</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>149783</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6649,13 +6658,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>469153</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>75826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>56029</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>-1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6718,13 +6727,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>224117</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>124385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>205442</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6787,13 +6796,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>448235</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>126067</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>214781</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>124385</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6843,13 +6852,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>566084</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>126067</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>418353</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>75826</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6899,13 +6908,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28761</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>37912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>469153</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6955,13 +6964,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>375770</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>178547</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>74706</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>80682</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7018,13 +7027,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>225237</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>98253</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>422590</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>178548</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7076,13 +7085,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>199466</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>552452</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7140,13 +7149,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>20357</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>5603</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>269214</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7199,13 +7208,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>386791</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>101039</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>146985</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>127187</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7263,13 +7272,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>224118</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>110940</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>298823</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>28016</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7998,13 +8007,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C65F3B7-4679-46BB-9C6C-4439D434827C}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8040,132 +8049,132 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>45127</v>
+        <v>45129</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>45126</v>
+        <v>45128</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>45125</v>
+        <v>45127</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>45124</v>
+        <v>45126</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>45123</v>
+        <v>45125</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
+        <v>45124</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>45123</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>45122</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B9" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>36</v>
-      </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
-        <v>45121</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
-        <v>45120</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <v>45119</v>
+        <v>45121</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>45118</v>
+        <v>45120</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>45117</v>
+        <v>45119</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
@@ -8174,10 +8183,10 @@
     </row>
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>45116</v>
+        <v>45118</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
@@ -8186,34 +8195,34 @@
     </row>
     <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>45115</v>
+        <v>45117</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <v>45114</v>
+        <v>45116</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>45113</v>
+        <v>45115</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
         <v>33</v>
@@ -8222,289 +8231,313 @@
     </row>
     <row r="17" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>45112</v>
+        <v>45114</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>45111</v>
+        <v>45113</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>45110</v>
+        <v>45112</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>45108</v>
+        <v>45110</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
+        <v>78</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
+        <v>45109</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>45108</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
         <v>45107</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B24" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="4">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
         <v>45106</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="4">
-        <v>45105</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="4">
-        <v>45106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="4">
-        <v>45104</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="C25" t="s">
         <v>33</v>
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
-        <v>45103</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>65</v>
+        <v>45105</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="D26" s="4">
+        <v>45106</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
-        <v>45102</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>43</v>
+        <v>45104</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="4">
-        <v>45110</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
-        <v>45102</v>
+        <v>45103</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="4">
-        <v>45117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
-        <v>45101</v>
+        <v>45102</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
         <v>36</v>
       </c>
+      <c r="D29" s="4">
+        <v>45110</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
+        <v>45102</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="4">
+        <v>45117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="4">
         <v>45101</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="9"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="10">
-        <v>45101</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>45101</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>33</v>
       </c>
+      <c r="D32" s="9"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" t="s">
+    <row r="33" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="10">
+        <v>45101</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="4">
+        <v>45101</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>45100</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>34</v>
+      <c r="B35" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="C35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>45100</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>45100</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>45100</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
-        <v>45099</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>25</v>
+        <v>45100</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="C39" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4">
         <v>45099</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B41" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="4">
+        <v>45099</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:D1048576 G29:G32">
+  <conditionalFormatting sqref="G31:G34 C1:D1048576">
     <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
@@ -10032,15 +10065,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FF080-9AD9-4A26-A8C8-2A6C2F748CFF}">
-  <dimension ref="A1:Z48"/>
+  <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView zoomScale="68" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -10050,7 +10083,9 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="J1" s="22" t="s">
+        <v>126</v>
+      </c>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
@@ -10064,6 +10099,9 @@
       <c r="U1" s="12"/>
       <c r="V1" s="12"/>
       <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
@@ -10089,6 +10127,9 @@
       <c r="U2" s="12"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="12"/>
@@ -10114,6 +10155,9 @@
       <c r="U3" s="12"/>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
@@ -10196,9 +10240,7 @@
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
-      <c r="Y6" s="12" t="s">
-        <v>126</v>
-      </c>
+      <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
@@ -10226,9 +10268,7 @@
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
       <c r="X7" s="12"/>
-      <c r="Y7" s="12" t="s">
-        <v>127</v>
-      </c>
+      <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
@@ -10256,9 +10296,7 @@
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
-      <c r="Y8" s="12" t="s">
-        <v>128</v>
-      </c>
+      <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
@@ -11381,9 +11419,38 @@
       <c r="Y48" s="12"/>
       <c r="Z48" s="12"/>
     </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+      <c r="N49" s="12"/>
+      <c r="O49" s="12"/>
+      <c r="P49" s="12"/>
+      <c r="Q49" s="12"/>
+      <c r="R49" s="12"/>
+      <c r="S49" s="12"/>
+      <c r="T49" s="12"/>
+      <c r="U49" s="12"/>
+      <c r="V49" s="12"/>
+      <c r="W49" s="12"/>
+      <c r="X49" s="12"/>
+      <c r="Y49" s="12"/>
+      <c r="Z49" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated slides and questions
</commit_message>
<xml_diff>
--- a/Daily Project Journal.xlsx
+++ b/Daily Project Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\PythonAI\LearnH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29847FD5-4732-40E7-A2C8-A6EBDA06513F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1080E6D1-6D29-4996-BDD0-72B377835574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="877" activeTab="1" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="131">
   <si>
     <t>List of capabilities</t>
   </si>
@@ -531,6 +531,12 @@
   </si>
   <si>
     <t>Came up with CHEWIE. Filled in use cases.</t>
+  </si>
+  <si>
+    <t>Made new data capture and vectorDB with primary key in Estuary Flow and Pinecone. Sent Ankit use case deck.</t>
+  </si>
+  <si>
+    <t>Made list of 10-12 questions for interviewees.</t>
   </si>
 </sst>
 </file>
@@ -667,10 +673,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8007,13 +8013,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C65F3B7-4679-46BB-9C6C-4439D434827C}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8051,10 +8057,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>45129</v>
+        <v>45131</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -8063,142 +8069,142 @@
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>45128</v>
+        <v>45130</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>45127</v>
+        <v>45129</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>45126</v>
+        <v>45128</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>45125</v>
+        <v>45127</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>45124</v>
+        <v>45126</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>45123</v>
+        <v>45125</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
+        <v>45124</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>45123</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
         <v>45122</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B11" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>36</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
-        <v>45121</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
-        <v>45120</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>45119</v>
+        <v>45121</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>45118</v>
+        <v>45120</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>45117</v>
+        <v>45119</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="C14" t="s">
         <v>33</v>
@@ -8207,10 +8213,10 @@
     </row>
     <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <v>45116</v>
+        <v>45118</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C15" t="s">
         <v>33</v>
@@ -8219,263 +8225,265 @@
     </row>
     <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>45115</v>
+        <v>45117</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>45114</v>
+        <v>45116</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>45113</v>
+        <v>45115</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>45112</v>
+        <v>45114</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>45111</v>
+        <v>45113</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
+        <v>45112</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>45111</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
         <v>45110</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B23" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C23" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
         <v>45109</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B24" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C24" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="4">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
         <v>45108</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="4">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="4">
         <v>45107</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B26" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="4">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
         <v>45106</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B27" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="4">
-        <v>45105</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="4">
-        <v>45106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="4">
-        <v>45104</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="C27" t="s">
         <v>33</v>
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
+        <v>45105</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="4">
+        <v>45106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="4">
+        <v>45104</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="4">
         <v>45103</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="C28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="4">
-        <v>45102</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="4">
-        <v>45110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="4">
-        <v>45102</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="C30" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="4">
-        <v>45117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
-        <v>45101</v>
+        <v>45102</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D31" s="4">
+        <v>45110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
+        <v>45102</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="4">
+        <v>45117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="4">
         <v>45101</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="9"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="10">
-        <v>45101</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B33" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>45101</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>33</v>
       </c>
+      <c r="D34" s="9"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" t="s">
+    <row r="35" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="10">
+        <v>45101</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="4">
+        <v>45101</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
+      <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>45100</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>34</v>
+      <c r="B37" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="C37" t="s">
         <v>33</v>
@@ -8486,10 +8494,10 @@
         <v>45100</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -8497,7 +8505,7 @@
         <v>45100</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
         <v>33</v>
@@ -8508,7 +8516,7 @@
         <v>45100</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
         <v>36</v>
@@ -8516,10 +8524,10 @@
     </row>
     <row r="41" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
-        <v>45099</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>25</v>
+        <v>45100</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="C41" t="s">
         <v>33</v>
@@ -8527,17 +8535,39 @@
     </row>
     <row r="42" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="4">
         <v>45099</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B43" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4">
+        <v>45099</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G31:G34 C1:D1048576">
+  <conditionalFormatting sqref="G33:G36 C1:D1048576">
     <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
@@ -8723,10 +8753,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -8745,10 +8775,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="22"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -10083,7 +10113,7 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>126</v>
       </c>
       <c r="K1" s="12"/>

</xml_diff>